<commit_message>
datasets added to database with sql db export
</commit_message>
<xml_diff>
--- a/dataset/excel/privilege-networks.xlsx
+++ b/dataset/excel/privilege-networks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aswin\Documents\Project-Documentation\Contextually Self-Organising Maps for Driving Risk Avoidance\dataset\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786329E5-2806-4A50-A7ED-8257A7642F14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C65E3BE-F856-4538-8632-9CF00BA4DA96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1FF153BD-2F54-413B-BC44-4030A878A0EB}"/>
   </bookViews>
@@ -621,7 +621,7 @@
   <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>